<commit_message>
updated qmd, md, docx, code, images
</commit_message>
<xml_diff>
--- a/pricingcomparison.xlsx
+++ b/pricingcomparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ainapudi/Desktop/multimodal-rag-on-slide-decks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8306C8-91EF-CA4F-B373-3ADBE89047D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACA84F5F-D50A-514E-B1AE-4CDFA0C17D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19240" xr2:uid="{BEBA8347-5D96-5440-96D2-646A5128C4D4}"/>
   </bookViews>
@@ -576,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B723AB-3729-164F-A81B-11EED7E96CFC}">
   <dimension ref="B3:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="162" zoomScaleNormal="162" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="162" zoomScaleNormal="162" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>